<commit_message>
add Sample file to the updated file
</commit_message>
<xml_diff>
--- a/OpenCart/testData/Opencart_LoginData.xlsx
+++ b/OpenCart/testData/Opencart_LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\15-Sept-2023batch\opencart\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\myworkspaces\seleniumwebdriver\OpencartV121\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3315BD60-ACC2-4D41-9A18-B0F87EEF7991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47704AFE-A492-43CB-82D7-6A46F57DC3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="17589" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="16354" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -168,9 +168,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,20 +485,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.23046875" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" customWidth="1"/>
-    <col min="3" max="3" width="18.15234375" customWidth="1"/>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -523,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -531,10 +528,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -542,10 +539,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -556,15 +553,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -576,8 +582,9 @@
     <hyperlink ref="B2" r:id="rId5" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
     <hyperlink ref="A6" r:id="rId6" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
     <hyperlink ref="B6" r:id="rId7" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{B4FF4FF2-C3C7-488B-A3F2-29DB9D3EA93F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>